<commit_message>
uploaded changes to risk assessment
</commit_message>
<xml_diff>
--- a/Project Files/Risk Assessment/Risk Assessment.xlsx
+++ b/Project Files/Risk Assessment/Risk Assessment.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\devel\ESS\Project Files\Risk Assessment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\devel\Engineering Software Systems\ESS\Project Files\Risk Assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08107F0-0773-4203-898A-98F8EC149E24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -108,12 +109,30 @@
   </si>
   <si>
     <t xml:space="preserve">University provides loads of machines should we lose access to our personal devices </t>
+  </si>
+  <si>
+    <t>Increased scope leading to loss of focus on core user requirements</t>
+  </si>
+  <si>
+    <t>Time constraints leading to user requirements not being fully met</t>
+  </si>
+  <si>
+    <t>Focus on core functionality defined in user requirements before continuing to add functionality</t>
+  </si>
+  <si>
+    <t>Ensure work is properly structured, using tools such as the Gantt chart</t>
+  </si>
+  <si>
+    <t>Feature Creep</t>
+  </si>
+  <si>
+    <t>Lack of consistency in work hours</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -160,11 +179,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -219,29 +239,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:G11" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:G11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:G11" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A1:G11" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="ID"/>
-    <tableColumn id="2" name="Risk event description and impact area"/>
-    <tableColumn id="3" name="Impact Rating"/>
-    <tableColumn id="4" name="Probability Rating"/>
-    <tableColumn id="5" name="Risk Score"/>
-    <tableColumn id="6" name="Risk Response Description"/>
-    <tableColumn id="7" name="Trigger"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Risk event description and impact area"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Impact Rating"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Probability Rating"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Risk Score"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Risk Response Description"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Trigger"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="I1:L5" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
-  <autoFilter ref="I1:L5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="I1:L8" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <autoFilter ref="I1:L8" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="If the impact to scope, cost, or customer is:" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="If the probability of the event occurring is: " dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Overall Risk Level is: " dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Risk Score " dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="If the impact to scope, cost, or customer is:" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="If the probability of the event occurring is: " dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Overall Risk Level is: " dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Risk Score " dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -509,21 +529,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="57.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.42578125" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" customWidth="1"/>
-    <col min="6" max="6" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="127.140625" customWidth="1"/>
+    <col min="7" max="7" width="42.42578125" customWidth="1"/>
     <col min="9" max="10" width="41.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.85546875" customWidth="1"/>
@@ -725,6 +746,88 @@
       </c>
       <c r="G6" t="s">
         <v>19</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="2">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>